<commit_message>
Patches & Script Commit
</commit_message>
<xml_diff>
--- a/doc/委托单任务单字段1.7.xlsx
+++ b/doc/委托单任务单字段1.7.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D10929E-1A81-4759-89EC-8279BEF4234E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F447C1-7D34-4C27-A70B-2785FE1B6491}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="任务单列表显示状态" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="446">
   <si>
     <t>委托单表头字段</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1624,10 +1624,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>NC_SAMPLE_INFO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC_SAMPLE_INFO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>纯文本</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>NC_SAMPLE_INFO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>手工填写，需校验是否符合规范</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1807,29 +1819,6 @@
   <si>
     <t>NC_SAMPLE_GROUP.PK_SAMPLE_GROUP</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NC_BASPROD_TYPE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NC_BASEN_TYPE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NC_BASPROD_POINT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NC_BASPROD_STRUCT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NC_BASPROD_CONTACT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NC_BASPROD_TEMP</t>
   </si>
 </sst>
 </file>
@@ -2141,31 +2130,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2177,16 +2142,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2197,6 +2171,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2503,20 +2492,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="27.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="27" t="s">
         <v>352</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
     </row>
     <row r="3" spans="2:13" ht="28" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
@@ -2732,26 +2721,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
     </row>
     <row r="3" spans="1:18" ht="42" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
@@ -2805,41 +2794,41 @@
     </row>
     <row r="4" spans="1:18" ht="28" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>407</v>
+      <c r="D4" s="31" t="s">
+        <v>410</v>
       </c>
       <c r="E4" s="24"/>
       <c r="F4" s="24"/>
       <c r="G4" s="24"/>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="J4" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="K4" s="30" t="s">
+      <c r="K4" s="27" t="s">
         <v>303</v>
       </c>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30" t="s">
+      <c r="L4" s="27"/>
+      <c r="M4" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="30" t="s">
+      <c r="N4" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="O4" s="30" t="s">
+      <c r="O4" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="P4" s="30"/>
+      <c r="P4" s="27"/>
       <c r="Q4" s="12" t="s">
         <v>36</v>
       </c>
@@ -2849,21 +2838,21 @@
     </row>
     <row r="5" spans="1:18" ht="28" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="34"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
       <c r="Q5" s="12" t="s">
         <v>37</v>
       </c>
@@ -3057,39 +3046,39 @@
     </row>
     <row r="11" spans="1:18" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="31" t="s">
         <v>378</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11" s="24"/>
       <c r="G11" s="24"/>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="27" t="s">
         <v>349</v>
       </c>
-      <c r="I11" s="32" t="s">
+      <c r="I11" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="J11" s="30" t="s">
+      <c r="J11" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="K11" s="30" t="s">
+      <c r="K11" s="27" t="s">
         <v>303</v>
       </c>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30" t="s">
+      <c r="L11" s="27"/>
+      <c r="M11" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="N11" s="30" t="s">
+      <c r="N11" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30" t="s">
+      <c r="O11" s="27"/>
+      <c r="P11" s="27" t="s">
         <v>28</v>
       </c>
       <c r="Q11" s="12" t="s">
@@ -3099,21 +3088,21 @@
     </row>
     <row r="12" spans="1:18" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="34"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="32"/>
       <c r="E12" s="25"/>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
       <c r="Q12" s="12" t="s">
         <v>39</v>
       </c>
@@ -3267,39 +3256,39 @@
     </row>
     <row r="17" spans="1:18" ht="28" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="31" t="s">
         <v>380</v>
       </c>
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
       <c r="G17" s="24"/>
-      <c r="H17" s="30" t="s">
+      <c r="H17" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="I17" s="32" t="s">
+      <c r="I17" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="J17" s="30" t="s">
+      <c r="J17" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="K17" s="30" t="s">
+      <c r="K17" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30" t="s">
+      <c r="L17" s="27"/>
+      <c r="M17" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="N17" s="30" t="s">
+      <c r="N17" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="O17" s="30"/>
-      <c r="P17" s="30"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
       <c r="Q17" s="12" t="s">
         <v>41</v>
       </c>
@@ -3309,21 +3298,21 @@
     </row>
     <row r="18" spans="1:18" ht="28" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="35"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
       <c r="G18" s="26"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
       <c r="Q18" s="12" t="s">
         <v>42</v>
       </c>
@@ -3333,37 +3322,37 @@
     </row>
     <row r="19" spans="1:18" ht="28" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="35"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="26"/>
       <c r="F19" s="26"/>
       <c r="G19" s="26"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="I19" s="32" t="s">
+      <c r="I19" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="J19" s="30" t="s">
+      <c r="J19" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="K19" s="30" t="s">
+      <c r="K19" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30" t="s">
+      <c r="L19" s="27"/>
+      <c r="M19" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="N19" s="30"/>
-      <c r="O19" s="30" t="s">
+      <c r="N19" s="27"/>
+      <c r="O19" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="P19" s="30"/>
+      <c r="P19" s="27"/>
       <c r="Q19" s="12" t="s">
         <v>44</v>
       </c>
@@ -3373,21 +3362,21 @@
     </row>
     <row r="20" spans="1:18" ht="28" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="35"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="33"/>
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
       <c r="Q20" s="12" t="s">
         <v>45</v>
       </c>
@@ -3397,35 +3386,35 @@
     </row>
     <row r="21" spans="1:18" ht="28" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="35"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="26"/>
       <c r="F21" s="26"/>
       <c r="G21" s="26"/>
-      <c r="H21" s="30" t="s">
+      <c r="H21" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="I21" s="32" t="s">
+      <c r="I21" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="J21" s="30" t="s">
+      <c r="J21" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="K21" s="30" t="s">
+      <c r="K21" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30" t="s">
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="P21" s="30"/>
+      <c r="P21" s="27"/>
       <c r="Q21" s="12" t="s">
         <v>49</v>
       </c>
@@ -3435,21 +3424,21 @@
     </row>
     <row r="22" spans="1:18" ht="28" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="34"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="32"/>
       <c r="E22" s="25"/>
       <c r="F22" s="25"/>
       <c r="G22" s="25"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="30"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
       <c r="Q22" s="12" t="s">
         <v>50</v>
       </c>
@@ -3534,7 +3523,7 @@
       <c r="R24" s="12"/>
     </row>
     <row r="25" spans="1:18" ht="28" x14ac:dyDescent="0.3">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="27" t="s">
         <v>301</v>
       </c>
       <c r="B25" s="12" t="s">
@@ -3543,7 +3532,7 @@
       <c r="C25" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="36" t="s">
+      <c r="D25" s="28" t="s">
         <v>384</v>
       </c>
       <c r="E25" s="13"/>
@@ -3566,14 +3555,14 @@
       <c r="R25" s="12"/>
     </row>
     <row r="26" spans="1:18" ht="28" x14ac:dyDescent="0.3">
-      <c r="A26" s="30"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="37"/>
+      <c r="D26" s="29"/>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
       <c r="G26" s="21"/>
@@ -3594,14 +3583,14 @@
       <c r="R26" s="12"/>
     </row>
     <row r="27" spans="1:18" ht="28" x14ac:dyDescent="0.3">
-      <c r="A27" s="30"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="12" t="s">
         <v>56</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="37"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
@@ -3622,14 +3611,14 @@
       <c r="R27" s="12"/>
     </row>
     <row r="28" spans="1:18" ht="28" x14ac:dyDescent="0.3">
-      <c r="A28" s="30"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="12" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="37"/>
+      <c r="D28" s="29"/>
       <c r="E28" s="21"/>
       <c r="F28" s="21"/>
       <c r="G28" s="21"/>
@@ -3650,14 +3639,14 @@
       <c r="R28" s="12"/>
     </row>
     <row r="29" spans="1:18" ht="28" x14ac:dyDescent="0.3">
-      <c r="A29" s="30"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="12" t="s">
         <v>58</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="37"/>
+      <c r="D29" s="29"/>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
@@ -3678,14 +3667,14 @@
       <c r="R29" s="12"/>
     </row>
     <row r="30" spans="1:18" ht="28" x14ac:dyDescent="0.3">
-      <c r="A30" s="30"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="12" t="s">
         <v>60</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="37"/>
+      <c r="D30" s="29"/>
       <c r="E30" s="21"/>
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
@@ -3706,14 +3695,14 @@
       <c r="R30" s="12"/>
     </row>
     <row r="31" spans="1:18" ht="28" x14ac:dyDescent="0.3">
-      <c r="A31" s="30"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="12" t="s">
         <v>59</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="38"/>
+      <c r="D31" s="30"/>
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
@@ -3795,37 +3784,37 @@
     </row>
     <row r="34" spans="1:18" ht="28" x14ac:dyDescent="0.3">
       <c r="A34" s="12"/>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="31" t="s">
         <v>386</v>
       </c>
       <c r="E34" s="24"/>
       <c r="F34" s="24"/>
       <c r="G34" s="24"/>
-      <c r="H34" s="30" t="s">
+      <c r="H34" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="I34" s="32" t="s">
+      <c r="I34" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="J34" s="30" t="s">
+      <c r="J34" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="K34" s="30" t="s">
+      <c r="K34" s="27" t="s">
         <v>303</v>
       </c>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30" t="s">
+      <c r="L34" s="27"/>
+      <c r="M34" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="N34" s="30"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="30" t="s">
+      <c r="N34" s="27"/>
+      <c r="O34" s="27"/>
+      <c r="P34" s="27" t="s">
         <v>82</v>
       </c>
       <c r="Q34" s="12" t="s">
@@ -3835,21 +3824,21 @@
     </row>
     <row r="35" spans="1:18" ht="28" x14ac:dyDescent="0.3">
       <c r="A35" s="12"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="34"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="32"/>
       <c r="E35" s="25"/>
       <c r="F35" s="25"/>
       <c r="G35" s="25"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="30"/>
-      <c r="O35" s="30"/>
-      <c r="P35" s="30"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
+      <c r="L35" s="27"/>
+      <c r="M35" s="27"/>
+      <c r="N35" s="27"/>
+      <c r="O35" s="27"/>
+      <c r="P35" s="27"/>
       <c r="Q35" s="12" t="s">
         <v>76</v>
       </c>
@@ -4274,16 +4263,16 @@
       <c r="G49" s="11"/>
     </row>
     <row r="50" spans="2:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="31"/>
-      <c r="I50" s="31"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D51" s="11"/>
@@ -4461,26 +4450,41 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="N34:N35"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D17:D22"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="M34:M35"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="D25:D31"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="O34:O35"/>
+    <mergeCell ref="B50:I50"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="H17:H18"/>
     <mergeCell ref="A2:R2"/>
     <mergeCell ref="A25:A31"/>
     <mergeCell ref="N11:N12"/>
@@ -4497,44 +4501,29 @@
     <mergeCell ref="O19:O20"/>
     <mergeCell ref="O21:O22"/>
     <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D17:D22"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="M34:M35"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="M17:M18"/>
     <mergeCell ref="O17:O18"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="P34:P35"/>
-    <mergeCell ref="O34:O35"/>
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="D25:D31"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="N34:N35"/>
+    <mergeCell ref="I21:I22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4547,8 +4536,8 @@
   <dimension ref="B2:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4586,17 +4575,17 @@
       <c r="D3" s="23" t="s">
         <v>376</v>
       </c>
-      <c r="E3" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>411</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>412</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>423</v>
+      <c r="E3" s="41" t="s">
+        <v>413</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>414</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>415</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>426</v>
       </c>
       <c r="I3" s="12" t="s">
         <v>3</v>
@@ -4627,128 +4616,128 @@
       </c>
     </row>
     <row r="4" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>443</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>421</v>
-      </c>
-      <c r="F4" s="39" t="s">
-        <v>420</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>419</v>
-      </c>
-      <c r="H4" s="28" t="s">
+      <c r="D4" s="31" t="s">
+        <v>396</v>
+      </c>
+      <c r="E4" s="42" t="s">
         <v>424</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="F4" s="42" t="s">
+        <v>423</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>422</v>
+      </c>
+      <c r="H4" s="43" t="s">
+        <v>427</v>
+      </c>
+      <c r="I4" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="J4" s="32" t="s">
+      <c r="J4" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="K4" s="30" t="s">
+      <c r="K4" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="27" t="s">
         <v>303</v>
       </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30" t="s">
+      <c r="M4" s="27"/>
+      <c r="N4" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="30" t="s">
+      <c r="O4" s="27" t="s">
         <v>87</v>
       </c>
       <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
     </row>
     <row r="5" spans="2:17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
       <c r="P5" s="12" t="s">
         <v>86</v>
       </c>
       <c r="Q5" s="12"/>
     </row>
     <row r="6" spans="2:17" ht="42" x14ac:dyDescent="0.3">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="33" t="s">
-        <v>444</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>415</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>414</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>416</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>425</v>
-      </c>
-      <c r="I6" s="30" t="s">
+      <c r="D6" s="31" t="s">
+        <v>397</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>418</v>
+      </c>
+      <c r="F6" s="43" t="s">
+        <v>417</v>
+      </c>
+      <c r="G6" s="43" t="s">
+        <v>419</v>
+      </c>
+      <c r="H6" s="43" t="s">
+        <v>428</v>
+      </c>
+      <c r="I6" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="K6" s="30" t="s">
+      <c r="K6" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="L6" s="30" t="s">
+      <c r="L6" s="27" t="s">
         <v>303</v>
       </c>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30" t="s">
+      <c r="M6" s="27"/>
+      <c r="N6" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="O6" s="30" t="s">
+      <c r="O6" s="27" t="s">
         <v>220</v>
       </c>
       <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
     </row>
     <row r="7" spans="2:17" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
       <c r="P7" s="12" t="s">
         <v>88</v>
       </c>
@@ -4762,12 +4751,12 @@
         <v>23</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>396</v>
-      </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+        <v>398</v>
+      </c>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12" t="s">
         <v>231</v>
@@ -4785,44 +4774,44 @@
       <c r="Q8" s="12"/>
     </row>
     <row r="9" spans="2:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="33" t="s">
-        <v>445</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>422</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>417</v>
-      </c>
-      <c r="G9" s="28" t="s">
-        <v>418</v>
-      </c>
-      <c r="H9" s="28" t="s">
-        <v>426</v>
-      </c>
-      <c r="I9" s="30" t="s">
+      <c r="D9" s="31" t="s">
+        <v>396</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>425</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>420</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>421</v>
+      </c>
+      <c r="H9" s="43" t="s">
+        <v>429</v>
+      </c>
+      <c r="I9" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="J9" s="36" t="s">
+      <c r="J9" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="K9" s="30" t="s">
+      <c r="K9" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="27" t="s">
         <v>303</v>
       </c>
-      <c r="M9" s="30"/>
-      <c r="N9" s="36" t="s">
+      <c r="M9" s="27"/>
+      <c r="N9" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="O9" s="30" t="s">
+      <c r="O9" s="27" t="s">
         <v>103</v>
       </c>
       <c r="P9" s="12" t="s">
@@ -4831,64 +4820,64 @@
       <c r="Q9" s="12"/>
     </row>
     <row r="10" spans="2:17" ht="126" x14ac:dyDescent="0.3">
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29" t="s">
-        <v>427</v>
-      </c>
-      <c r="I10" s="30"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="30"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45" t="s">
+        <v>430</v>
+      </c>
+      <c r="I10" s="27"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="27"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="33" t="s">
-        <v>446</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>429</v>
-      </c>
-      <c r="F11" s="39" t="s">
-        <v>430</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>428</v>
-      </c>
-      <c r="H11" s="28" t="s">
-        <v>438</v>
-      </c>
-      <c r="I11" s="30" t="s">
+      <c r="D11" s="31" t="s">
+        <v>399</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>432</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>433</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>431</v>
+      </c>
+      <c r="H11" s="43" t="s">
+        <v>441</v>
+      </c>
+      <c r="I11" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="J11" s="36" t="s">
+      <c r="J11" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="K11" s="30" t="s">
+      <c r="K11" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="L11" s="30" t="s">
+      <c r="L11" s="27" t="s">
         <v>303</v>
       </c>
-      <c r="M11" s="30"/>
-      <c r="N11" s="36" t="s">
+      <c r="M11" s="27"/>
+      <c r="N11" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="O11" s="30" t="s">
+      <c r="O11" s="27" t="s">
         <v>104</v>
       </c>
       <c r="P11" s="12" t="s">
@@ -4897,62 +4886,62 @@
       <c r="Q11" s="12"/>
     </row>
     <row r="12" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="30"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="27"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
     </row>
     <row r="13" spans="2:17" ht="42" x14ac:dyDescent="0.3">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="33" t="s">
-        <v>447</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>431</v>
-      </c>
-      <c r="F13" s="39" t="s">
-        <v>432</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>433</v>
-      </c>
-      <c r="H13" s="28" t="s">
+      <c r="D13" s="31" t="s">
+        <v>397</v>
+      </c>
+      <c r="E13" s="42" t="s">
         <v>434</v>
       </c>
-      <c r="I13" s="30" t="s">
+      <c r="F13" s="42" t="s">
+        <v>435</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>436</v>
+      </c>
+      <c r="H13" s="43" t="s">
+        <v>437</v>
+      </c>
+      <c r="I13" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="J13" s="41" t="s">
+      <c r="J13" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="K13" s="30" t="s">
+      <c r="K13" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="L13" s="30" t="s">
+      <c r="L13" s="27" t="s">
         <v>303</v>
       </c>
-      <c r="M13" s="30"/>
-      <c r="N13" s="36" t="s">
+      <c r="M13" s="27"/>
+      <c r="N13" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="O13" s="30" t="s">
+      <c r="O13" s="27" t="s">
         <v>105</v>
       </c>
       <c r="P13" s="12" t="s">
@@ -4961,20 +4950,20 @@
       <c r="Q13" s="12"/>
     </row>
     <row r="14" spans="2:17" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="30"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="27"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
     </row>
@@ -4986,12 +4975,12 @@
         <v>100</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>397</v>
-      </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
+        <v>400</v>
+      </c>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
       <c r="I15" s="12"/>
       <c r="J15" s="15" t="s">
         <v>189</v>
@@ -5007,112 +4996,112 @@
       <c r="Q15" s="12"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="33" t="s">
-        <v>399</v>
-      </c>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="41" t="s">
+      <c r="D16" s="31" t="s">
+        <v>402</v>
+      </c>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30" t="s">
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="O16" s="30"/>
+      <c r="O16" s="27"/>
       <c r="P16" s="12" t="s">
         <v>108</v>
       </c>
       <c r="Q16" s="12"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
       <c r="P17" s="12" t="s">
         <v>109</v>
       </c>
       <c r="Q17" s="12"/>
     </row>
     <row r="18" spans="2:17" ht="42" x14ac:dyDescent="0.3">
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="33" t="s">
-        <v>398</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>409</v>
-      </c>
-      <c r="F18" s="28" t="s">
-        <v>408</v>
-      </c>
-      <c r="G18" s="28" t="s">
-        <v>413</v>
-      </c>
-      <c r="H18" s="28"/>
-      <c r="I18" s="30" t="s">
+      <c r="D18" s="31" t="s">
+        <v>401</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="F18" s="43" t="s">
+        <v>411</v>
+      </c>
+      <c r="G18" s="43" t="s">
+        <v>416</v>
+      </c>
+      <c r="H18" s="43"/>
+      <c r="I18" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="J18" s="41" t="s">
+      <c r="J18" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="K18" s="30" t="s">
+      <c r="K18" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="L18" s="30" t="s">
+      <c r="L18" s="27" t="s">
         <v>303</v>
       </c>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30" t="s">
+      <c r="M18" s="27"/>
+      <c r="N18" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="O18" s="30"/>
+      <c r="O18" s="27"/>
       <c r="P18" s="12" t="s">
         <v>106</v>
       </c>
       <c r="Q18" s="12"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="30"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="27"/>
       <c r="P19" s="12" t="s">
         <v>107</v>
       </c>
@@ -5126,12 +5115,12 @@
         <v>23</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>400</v>
-      </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
+        <v>403</v>
+      </c>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
       <c r="I20" s="12"/>
       <c r="J20" s="15" t="s">
         <v>192</v>
@@ -5156,19 +5145,19 @@
         <v>25</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>448</v>
-      </c>
-      <c r="E21" s="27" t="s">
-        <v>435</v>
-      </c>
-      <c r="F21" s="27" t="s">
-        <v>436</v>
-      </c>
-      <c r="G21" s="27" t="s">
-        <v>437</v>
-      </c>
-      <c r="H21" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>438</v>
+      </c>
+      <c r="F21" s="41" t="s">
         <v>439</v>
+      </c>
+      <c r="G21" s="41" t="s">
+        <v>440</v>
+      </c>
+      <c r="H21" s="41" t="s">
+        <v>442</v>
       </c>
       <c r="I21" s="12" t="s">
         <v>186</v>
@@ -5202,18 +5191,18 @@
         <v>25</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>401</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>440</v>
-      </c>
-      <c r="F22" s="27" t="s">
-        <v>441</v>
-      </c>
-      <c r="G22" s="27" t="s">
-        <v>442</v>
-      </c>
-      <c r="H22" s="27"/>
+        <v>404</v>
+      </c>
+      <c r="E22" s="41" t="s">
+        <v>443</v>
+      </c>
+      <c r="F22" s="41" t="s">
+        <v>444</v>
+      </c>
+      <c r="G22" s="41" t="s">
+        <v>445</v>
+      </c>
+      <c r="H22" s="41"/>
       <c r="I22" s="12" t="s">
         <v>144</v>
       </c>
@@ -5244,12 +5233,12 @@
         <v>25</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>403</v>
-      </c>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
+        <v>406</v>
+      </c>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
       <c r="I23" s="12" t="s">
         <v>213</v>
       </c>
@@ -5274,12 +5263,12 @@
         <v>23</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>396</v>
-      </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
+        <v>398</v>
+      </c>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
       <c r="I24" s="12"/>
       <c r="J24" s="15" t="s">
         <v>194</v>
@@ -5295,29 +5284,73 @@
       <c r="Q24" s="12"/>
     </row>
     <row r="26" spans="2:17" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="35" t="s">
         <v>212</v>
       </c>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="M11:M12"/>
     <mergeCell ref="N11:N12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="O6:O7"/>
@@ -5334,60 +5367,16 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="M6:M7"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="C26:J26"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5482,7 +5471,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>214</v>
@@ -5511,8 +5500,8 @@
       <c r="C6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="33" t="s">
-        <v>404</v>
+      <c r="D6" s="31" t="s">
+        <v>407</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>215</v>
@@ -5542,7 +5531,7 @@
         <v>371</v>
       </c>
       <c r="C7" s="12"/>
-      <c r="D7" s="35"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -5559,7 +5548,7 @@
       <c r="C8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="33"/>
       <c r="E8" s="12" t="s">
         <v>218</v>
       </c>
@@ -5585,7 +5574,7 @@
       <c r="C9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="35"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="12" t="s">
         <v>219</v>
       </c>
@@ -5611,7 +5600,7 @@
       <c r="C10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="35"/>
+      <c r="D10" s="33"/>
       <c r="E10" s="12" t="s">
         <v>216</v>
       </c>
@@ -5637,7 +5626,7 @@
       <c r="C11" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="D11" s="35"/>
+      <c r="D11" s="33"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12" t="s">
         <v>226</v>
@@ -5661,7 +5650,7 @@
       <c r="C12" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="D12" s="35"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12" t="s">
         <v>227</v>
@@ -5685,7 +5674,7 @@
       <c r="C13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="34"/>
+      <c r="D13" s="32"/>
       <c r="E13" s="12" t="s">
         <v>217</v>
       </c>
@@ -5735,19 +5724,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
     </row>
     <row r="3" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
@@ -5791,8 +5780,8 @@
       <c r="C4" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>405</v>
+      <c r="D4" s="31" t="s">
+        <v>408</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -5806,40 +5795,40 @@
       <c r="L4" s="12"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="30" t="s">
+      <c r="D5" s="33"/>
+      <c r="E5" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30" t="s">
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="30" t="s">
+      <c r="K5" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="L5" s="30"/>
+      <c r="L5" s="27"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
     </row>
     <row r="7" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
@@ -5848,7 +5837,7 @@
       <c r="C7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="35"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -5869,7 +5858,7 @@
       <c r="C8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="33"/>
       <c r="E8" s="12" t="s">
         <v>123</v>
       </c>
@@ -5892,7 +5881,7 @@
       <c r="C9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="35"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="12" t="s">
         <v>126</v>
       </c>
@@ -5913,7 +5902,7 @@
       <c r="C10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="35"/>
+      <c r="D10" s="33"/>
       <c r="E10" s="12" t="s">
         <v>128</v>
       </c>
@@ -5936,7 +5925,7 @@
       <c r="C11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="35"/>
+      <c r="D11" s="33"/>
       <c r="E11" s="12" t="s">
         <v>129</v>
       </c>
@@ -5953,38 +5942,38 @@
       <c r="L11" s="12"/>
     </row>
     <row r="12" spans="2:12" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="30" t="s">
+      <c r="D12" s="33"/>
+      <c r="E12" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30" t="s">
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
     </row>
     <row r="14" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
@@ -5993,7 +5982,7 @@
       <c r="C14" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="35"/>
+      <c r="D14" s="33"/>
       <c r="E14" s="12" t="s">
         <v>130</v>
       </c>
@@ -6016,7 +6005,7 @@
       <c r="C15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="35"/>
+      <c r="D15" s="33"/>
       <c r="E15" s="12" t="s">
         <v>131</v>
       </c>
@@ -6037,7 +6026,7 @@
       <c r="C16" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="35"/>
+      <c r="D16" s="33"/>
       <c r="E16" s="12" t="s">
         <v>134</v>
       </c>
@@ -6060,7 +6049,7 @@
       <c r="C17" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="35"/>
+      <c r="D17" s="33"/>
       <c r="E17" s="12" t="s">
         <v>135</v>
       </c>
@@ -6077,108 +6066,108 @@
       <c r="L17" s="12"/>
     </row>
     <row r="18" spans="2:12" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="30" t="s">
+      <c r="D18" s="33"/>
+      <c r="E18" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30" t="s">
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
     </row>
     <row r="20" spans="2:12" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="30" t="s">
+      <c r="D20" s="33"/>
+      <c r="E20" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30" t="s">
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="K20" s="30" t="s">
+      <c r="K20" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="L20" s="30"/>
+      <c r="L20" s="27"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="30" t="s">
+      <c r="D22" s="33"/>
+      <c r="E22" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30" t="s">
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="L22" s="30"/>
+      <c r="L22" s="27"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="12" t="s">
@@ -6187,7 +6176,7 @@
       <c r="C24" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="35"/>
+      <c r="D24" s="33"/>
       <c r="E24" s="12" t="s">
         <v>146</v>
       </c>
@@ -6208,7 +6197,7 @@
       <c r="C25" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="35"/>
+      <c r="D25" s="33"/>
       <c r="E25" s="12" t="s">
         <v>147</v>
       </c>
@@ -6229,7 +6218,7 @@
       <c r="C26" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="35"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="12" t="s">
         <v>164</v>
       </c>
@@ -6250,7 +6239,7 @@
       <c r="C27" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="35"/>
+      <c r="D27" s="33"/>
       <c r="E27" s="12" t="s">
         <v>165</v>
       </c>
@@ -6265,40 +6254,40 @@
       <c r="L27" s="12"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="30" t="s">
+      <c r="D28" s="33"/>
+      <c r="E28" s="27" t="s">
         <v>166</v>
       </c>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30" t="s">
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30" t="s">
+      <c r="K28" s="27"/>
+      <c r="L28" s="27" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
     </row>
     <row r="30" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B30" s="12" t="s">
@@ -6307,7 +6296,7 @@
       <c r="C30" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="35"/>
+      <c r="D30" s="33"/>
       <c r="E30" s="12" t="s">
         <v>170</v>
       </c>
@@ -6326,7 +6315,7 @@
       <c r="C31" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="35"/>
+      <c r="D31" s="33"/>
       <c r="E31" s="12" t="s">
         <v>167</v>
       </c>
@@ -6347,7 +6336,7 @@
       <c r="C32" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="35"/>
+      <c r="D32" s="33"/>
       <c r="E32" s="12" t="s">
         <v>168</v>
       </c>
@@ -6366,7 +6355,7 @@
       <c r="C33" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="35"/>
+      <c r="D33" s="33"/>
       <c r="E33" s="12" t="s">
         <v>169</v>
       </c>
@@ -6385,7 +6374,7 @@
       <c r="C34" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D34" s="35"/>
+      <c r="D34" s="33"/>
       <c r="E34" s="12" t="s">
         <v>171</v>
       </c>
@@ -6404,7 +6393,7 @@
       <c r="C35" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="35"/>
+      <c r="D35" s="33"/>
       <c r="E35" s="12" t="s">
         <v>172</v>
       </c>
@@ -6425,7 +6414,7 @@
       <c r="C36" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="35"/>
+      <c r="D36" s="33"/>
       <c r="E36" s="12" t="s">
         <v>173</v>
       </c>
@@ -6446,7 +6435,7 @@
       <c r="C37" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="35"/>
+      <c r="D37" s="33"/>
       <c r="E37" s="12" t="s">
         <v>174</v>
       </c>
@@ -6467,7 +6456,7 @@
       <c r="C38" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="35"/>
+      <c r="D38" s="33"/>
       <c r="E38" s="12" t="s">
         <v>175</v>
       </c>
@@ -6488,7 +6477,7 @@
       <c r="C39" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="35"/>
+      <c r="D39" s="33"/>
       <c r="E39" s="12" t="s">
         <v>176</v>
       </c>
@@ -6507,7 +6496,7 @@
       <c r="C40" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D40" s="35"/>
+      <c r="D40" s="33"/>
       <c r="E40" s="12" t="s">
         <v>178</v>
       </c>
@@ -6526,7 +6515,7 @@
       <c r="C41" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D41" s="35"/>
+      <c r="D41" s="33"/>
       <c r="E41" s="12" t="s">
         <v>177</v>
       </c>
@@ -6545,7 +6534,7 @@
         <v>321</v>
       </c>
       <c r="C42" s="12"/>
-      <c r="D42" s="34"/>
+      <c r="D42" s="32"/>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
@@ -6557,6 +6546,52 @@
     </row>
   </sheetData>
   <mergeCells count="62">
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="H12:H13"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
@@ -6573,52 +6608,6 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6694,7 +6683,7 @@
         <v>202</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12" t="s">
@@ -6713,62 +6702,62 @@
       <c r="M3" s="12"/>
     </row>
     <row r="4" spans="2:13" ht="70" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="28" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="13"/>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="28" t="s">
         <v>255</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="28" t="s">
         <v>242</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="28" t="s">
         <v>280</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36" t="s">
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="36" t="s">
+      <c r="K4" s="28" t="s">
         <v>367</v>
       </c>
-      <c r="L4" s="36" t="s">
+      <c r="L4" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="M4" s="36" t="s">
+      <c r="M4" s="28" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="21"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
     </row>
     <row r="6" spans="2:13" ht="56" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="21"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
       <c r="L6" s="12" t="s">
         <v>211</v>
       </c>
@@ -6777,16 +6766,16 @@
       </c>
     </row>
     <row r="7" spans="2:13" ht="28" x14ac:dyDescent="0.3">
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
       <c r="L7" s="12" t="s">
         <v>258</v>
       </c>
@@ -6795,16 +6784,16 @@
       </c>
     </row>
     <row r="8" spans="2:13" ht="28" x14ac:dyDescent="0.3">
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
       <c r="L8" s="12" t="s">
         <v>260</v>
       </c>
@@ -6813,16 +6802,16 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="21"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
       <c r="L9" s="12" t="s">
         <v>262</v>
       </c>
@@ -6831,16 +6820,16 @@
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="22"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
       <c r="L10" s="12" t="s">
         <v>37</v>
       </c>
@@ -7726,10 +7715,10 @@
       <c r="J6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="44" t="s">
+      <c r="K6" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="45"/>
+      <c r="L6" s="40"/>
       <c r="M6" s="1" t="s">
         <v>9</v>
       </c>
@@ -7885,10 +7874,10 @@
       <c r="J16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="44" t="s">
+      <c r="K16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="L16" s="45"/>
+      <c r="L16" s="40"/>
       <c r="M16" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>